<commit_message>
some more famicon adv gamebooks
</commit_message>
<xml_diff>
--- a/famicon-adventure-gamebook/checklist.xlsx
+++ b/famicon-adventure-gamebook/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/famicon-adventure-gamebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14D4F4E3-8B17-F949-B9AC-0E451F7CED13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3572B1FD-ADA8-A549-9030-BA301179EC19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{34C05C4E-05DE-9C4D-BAF0-7EC06EA20153}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="215">
   <si>
     <t>year</t>
   </si>
@@ -448,6 +448,237 @@
   </si>
   <si>
     <t>murasame-castle.jpg</t>
+  </si>
+  <si>
+    <t>Super Mario Bros. Save Mario!</t>
+  </si>
+  <si>
+    <t>Super Mario Bros. Vol.2 Challenge of the Great Demon King Neo Kuppa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super Mario Bros. Vol.3 Mario Corps Sortie </t>
+  </si>
+  <si>
+    <t>Super Mario World Dinosaur Land Edition</t>
+  </si>
+  <si>
+    <t>The Legend of Zelda: Battle of Mirage Castle</t>
+  </si>
+  <si>
+    <t>Link's Adventure Counterattack from the Makai</t>
+  </si>
+  <si>
+    <t>The Legend of Zelda The Tri-force of the Gods</t>
+  </si>
+  <si>
+    <t>Dragon Quest The Legend of Heroes Revived</t>
+  </si>
+  <si>
+    <t>Dragon Quest II Evil Spirit Gods Part I</t>
+  </si>
+  <si>
+    <t>Dragon Quest II Evil Spirit Gods Part II</t>
+  </si>
+  <si>
+    <t>Battle with the Unknown Gradius</t>
+  </si>
+  <si>
+    <t>The Mysterious Murasame Castle Mysterious Age Trip</t>
+  </si>
+  <si>
+    <t>Castlevania Dracula Castlevania Death Fight</t>
+  </si>
+  <si>
+    <t>Castlevania legend authenticity Vampire Hunter</t>
+  </si>
+  <si>
+    <t>Rescue Takahashi Master's Adventure Island Tina!</t>
+  </si>
+  <si>
+    <t>Takahashi Meijin's Bug is a Honey Game World Crisis Close Call</t>
+  </si>
+  <si>
+    <t>Fantasy Zone Invaders from aliens</t>
+  </si>
+  <si>
+    <t>Fantasy Zone 2 Departure to an alien planet</t>
+  </si>
+  <si>
+    <t>Glory of Heracles The Legend of the Legend of the Young Hero</t>
+  </si>
+  <si>
+    <t>Glory of Heracles II New Hero</t>
+  </si>
+  <si>
+    <t>Momotaro Densetsu Exterminate Oni of Love and Courage</t>
+  </si>
+  <si>
+    <t>Momotaro Dentetsu Aim! President</t>
+  </si>
+  <si>
+    <t>Momotaro Lightning Stone Fire 00 Peach Close Call</t>
+  </si>
+  <si>
+    <t>Momotaro Densetsu Special Challenge the Snow Queen!</t>
+  </si>
+  <si>
+    <t>Momotaro swashbuckler Emma the Great's counterattack</t>
+  </si>
+  <si>
+    <t>Momotaro Densetsu II Hell King Appears!</t>
+  </si>
+  <si>
+    <t>Good luck Goemon! Karakuri Road Fifty-three Views of the Middle Tokaido</t>
+  </si>
+  <si>
+    <t>Good luck Goemon Gaiden Ichigo Senkin Treasure Ship</t>
+  </si>
+  <si>
+    <t>Good luck Goemon Yukihime rescue picture scroll</t>
+  </si>
+  <si>
+    <t>Ultima Mage Zor's Conspiracy</t>
+  </si>
+  <si>
+    <t>Ultima Vol.2 Road to the Saints</t>
+  </si>
+  <si>
+    <t>Boy Magician Indy Magical Inferno</t>
+  </si>
+  <si>
+    <t>Boy Wizard Indy 2 Forbidden Magical Power</t>
+  </si>
+  <si>
+    <t>Boy Wizard Indy 3 Foreign Wizard</t>
+  </si>
+  <si>
+    <t>Metroid Zebes Invasion Directive</t>
+  </si>
+  <si>
+    <t>Portopia Serial Murder Case The Mystery of Locked Room Murder</t>
+  </si>
+  <si>
+    <t>Murder on the Mississippi Riverboat Adventure</t>
+  </si>
+  <si>
+    <t>Tokoro-san's Mamoru Mosememo Akuaku Adventure</t>
+  </si>
+  <si>
+    <t>Sanma's Detective Bunchin Katsura Murder Case</t>
+  </si>
+  <si>
+    <t>Pocket Saurus Dinosaur Island Drifting Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getsu Fuma Den: Battle of the First Year of the Magic Calendar </t>
+  </si>
+  <si>
+    <t>Let's get rid of the Renegade Kunio-kun Bancho Union!</t>
+  </si>
+  <si>
+    <t>Kid Icarus Defeat the Devil in the Mirror Temple of Partena!</t>
+  </si>
+  <si>
+    <t>Argos Warrior Unsealed Seal</t>
+  </si>
+  <si>
+    <t>Future Myth Jarvas Chapter of the Messiah-Save the New Century!</t>
+  </si>
+  <si>
+    <t>Bomber King Altair Final War</t>
+  </si>
+  <si>
+    <t>Weiker's Magic Castle Totsugeki Makai Expedition</t>
+  </si>
+  <si>
+    <t>A new demon defeats the incarnation of the island darkness!</t>
+  </si>
+  <si>
+    <t>Faxanadu Dragon Fang</t>
+  </si>
+  <si>
+    <t>Pro Baseball Family Stadium Namco Stars Challenge</t>
+  </si>
+  <si>
+    <t>Professional Baseball Family Stadium Vol.2 Fengyun All-Star Game</t>
+  </si>
+  <si>
+    <t>Professional Baseball Family Stadium Vol.3 WE ARE THE CHAMPION!</t>
+  </si>
+  <si>
+    <t>Family Stadium '90 WE ARE THE WORLD!</t>
+  </si>
+  <si>
+    <t>Family Stadium Rainbow Reversal Arch</t>
+  </si>
+  <si>
+    <t>Wizardry Wizardry Wardna's Ambition</t>
+  </si>
+  <si>
+    <t>Wizardry II Le Kebres's Cave</t>
+  </si>
+  <si>
+    <t>Wizardry III Diamond Knight</t>
+  </si>
+  <si>
+    <t>Wizardry Gaiden I Queen's suffering</t>
+  </si>
+  <si>
+    <t>Famicom Tantei Club disappeared successor</t>
+  </si>
+  <si>
+    <t>Famicom Tantei Club PARTII Girl standing behind</t>
+  </si>
+  <si>
+    <t>Ys Dreadful Demon Tower</t>
+  </si>
+  <si>
+    <t>Ys II Demon King Revival</t>
+  </si>
+  <si>
+    <t>Ys III Legendary Demon King</t>
+  </si>
+  <si>
+    <t>FINAL FANTASY Light up the brave!</t>
+  </si>
+  <si>
+    <t>FINAL FANTASY II Hidden Dragon</t>
+  </si>
+  <si>
+    <t>ビックリマン 無縁ゾーンの秘宝</t>
+  </si>
+  <si>
+    <t>ビックリマン2　天聖門を開けろ！</t>
+  </si>
+  <si>
+    <t>surprise-man.jpg</t>
+  </si>
+  <si>
+    <t>surprise-man2.jpg</t>
+  </si>
+  <si>
+    <t>Bikkuriman Unrelated Zone Hallows</t>
+  </si>
+  <si>
+    <t>Surprise Man 2 Open the Tensei Gate!</t>
+  </si>
+  <si>
+    <t>魔神英雄伝ワタル 異次元の救世主</t>
+  </si>
+  <si>
+    <t>魔神英雄伝ワタル外伝 救世主再び!!</t>
+  </si>
+  <si>
+    <t>Mashin Hero Wataru, a savior of another dimension</t>
+  </si>
+  <si>
+    <t>Genie Hero Den Wataru Gaiden Savior Again !!</t>
+  </si>
+  <si>
+    <t>hero-wataru.jpg</t>
+  </si>
+  <si>
+    <t>hero-wataru2.jpg</t>
   </si>
 </sst>
 </file>
@@ -479,10 +710,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -491,9 +731,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,16 +1049,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B05840-0655-A245-99C3-6C443B4A591B}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="74" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
   </cols>
@@ -849,6 +1090,9 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -866,6 +1110,9 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>139</v>
+      </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
@@ -882,6 +1129,9 @@
       </c>
       <c r="B4" t="s">
         <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -900,6 +1150,9 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
@@ -917,6 +1170,9 @@
       <c r="B6" t="s">
         <v>19</v>
       </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
@@ -933,6 +1189,9 @@
       </c>
       <c r="B7" t="s">
         <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>143</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -951,6 +1210,9 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
+      <c r="C8" t="s">
+        <v>144</v>
+      </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
@@ -968,6 +1230,9 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
+      <c r="C9" t="s">
+        <v>145</v>
+      </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
@@ -985,6 +1250,9 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
+      <c r="C10" t="s">
+        <v>146</v>
+      </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
@@ -1001,6 +1269,9 @@
       </c>
       <c r="B11" t="s">
         <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>147</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1019,6 +1290,9 @@
       <c r="B12" t="s">
         <v>28</v>
       </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
@@ -1036,6 +1310,9 @@
       <c r="B13" t="s">
         <v>30</v>
       </c>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
@@ -1052,6 +1329,9 @@
       </c>
       <c r="B14" t="s">
         <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1070,6 +1350,9 @@
       <c r="B15" t="s">
         <v>33</v>
       </c>
+      <c r="C15" t="s">
+        <v>151</v>
+      </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
@@ -1087,6 +1370,9 @@
       <c r="B16" t="s">
         <v>38</v>
       </c>
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
@@ -1104,6 +1390,9 @@
       <c r="B17" t="s">
         <v>37</v>
       </c>
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
@@ -1120,6 +1409,9 @@
       </c>
       <c r="B18" t="s">
         <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>154</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -1138,6 +1430,9 @@
       <c r="B19" t="s">
         <v>41</v>
       </c>
+      <c r="C19" t="s">
+        <v>155</v>
+      </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
@@ -1154,6 +1449,9 @@
       </c>
       <c r="B20" t="s">
         <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>156</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -1172,6 +1470,9 @@
       <c r="B21" t="s">
         <v>44</v>
       </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
@@ -1188,6 +1489,9 @@
       </c>
       <c r="B22" t="s">
         <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>158</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -1206,6 +1510,9 @@
       <c r="B23" t="s">
         <v>48</v>
       </c>
+      <c r="C23" t="s">
+        <v>159</v>
+      </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
@@ -1223,6 +1530,9 @@
       <c r="B24" t="s">
         <v>49</v>
       </c>
+      <c r="C24" t="s">
+        <v>160</v>
+      </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
@@ -1240,6 +1550,9 @@
       <c r="B25" t="s">
         <v>50</v>
       </c>
+      <c r="C25" t="s">
+        <v>161</v>
+      </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
@@ -1257,6 +1570,9 @@
       <c r="B26" t="s">
         <v>51</v>
       </c>
+      <c r="C26" t="s">
+        <v>162</v>
+      </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
@@ -1274,6 +1590,9 @@
       <c r="B27" t="s">
         <v>52</v>
       </c>
+      <c r="C27" t="s">
+        <v>163</v>
+      </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
@@ -1290,6 +1609,9 @@
       </c>
       <c r="B28" t="s">
         <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>164</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1308,6 +1630,9 @@
       <c r="B29" t="s">
         <v>63</v>
       </c>
+      <c r="C29" t="s">
+        <v>165</v>
+      </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
@@ -1325,6 +1650,9 @@
       <c r="B30" t="s">
         <v>62</v>
       </c>
+      <c r="C30" t="s">
+        <v>166</v>
+      </c>
       <c r="D30" t="s">
         <v>10</v>
       </c>
@@ -1341,6 +1669,9 @@
       </c>
       <c r="B31" t="s">
         <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>167</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -1359,6 +1690,9 @@
       <c r="B32" t="s">
         <v>66</v>
       </c>
+      <c r="C32" t="s">
+        <v>168</v>
+      </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
@@ -1375,6 +1709,9 @@
       </c>
       <c r="B33" t="s">
         <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>169</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -1393,6 +1730,9 @@
       <c r="B34" t="s">
         <v>70</v>
       </c>
+      <c r="C34" t="s">
+        <v>170</v>
+      </c>
       <c r="D34" t="s">
         <v>10</v>
       </c>
@@ -1410,6 +1750,9 @@
       <c r="B35" t="s">
         <v>71</v>
       </c>
+      <c r="C35" t="s">
+        <v>171</v>
+      </c>
       <c r="D35" t="s">
         <v>10</v>
       </c>
@@ -1427,6 +1770,9 @@
       <c r="B36" t="s">
         <v>72</v>
       </c>
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
       <c r="D36" t="s">
         <v>10</v>
       </c>
@@ -1444,6 +1790,9 @@
       <c r="B37" t="s">
         <v>77</v>
       </c>
+      <c r="C37" t="s">
+        <v>173</v>
+      </c>
       <c r="D37" t="s">
         <v>10</v>
       </c>
@@ -1461,6 +1810,9 @@
       <c r="B38" t="s">
         <v>79</v>
       </c>
+      <c r="C38" t="s">
+        <v>174</v>
+      </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
@@ -1478,6 +1830,9 @@
       <c r="B39" t="s">
         <v>80</v>
       </c>
+      <c r="C39" t="s">
+        <v>180</v>
+      </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
@@ -1495,6 +1850,9 @@
       <c r="B40" t="s">
         <v>84</v>
       </c>
+      <c r="C40" t="s">
+        <v>175</v>
+      </c>
       <c r="D40" t="s">
         <v>10</v>
       </c>
@@ -1512,6 +1870,9 @@
       <c r="B41" t="s">
         <v>85</v>
       </c>
+      <c r="C41" t="s">
+        <v>176</v>
+      </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
@@ -1529,6 +1890,9 @@
       <c r="B42" t="s">
         <v>87</v>
       </c>
+      <c r="C42" t="s">
+        <v>177</v>
+      </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
@@ -1546,6 +1910,9 @@
       <c r="B43" t="s">
         <v>89</v>
       </c>
+      <c r="C43" t="s">
+        <v>178</v>
+      </c>
       <c r="D43" t="s">
         <v>10</v>
       </c>
@@ -1563,6 +1930,9 @@
       <c r="B44" t="s">
         <v>91</v>
       </c>
+      <c r="C44" t="s">
+        <v>179</v>
+      </c>
       <c r="D44" t="s">
         <v>10</v>
       </c>
@@ -1580,6 +1950,9 @@
       <c r="B45" t="s">
         <v>93</v>
       </c>
+      <c r="C45" t="s">
+        <v>181</v>
+      </c>
       <c r="D45" t="s">
         <v>10</v>
       </c>
@@ -1597,6 +1970,9 @@
       <c r="B46" t="s">
         <v>95</v>
       </c>
+      <c r="C46" t="s">
+        <v>182</v>
+      </c>
       <c r="D46" t="s">
         <v>10</v>
       </c>
@@ -1614,6 +1990,9 @@
       <c r="B47" t="s">
         <v>97</v>
       </c>
+      <c r="C47" t="s">
+        <v>183</v>
+      </c>
       <c r="D47" t="s">
         <v>10</v>
       </c>
@@ -1631,6 +2010,9 @@
       <c r="B48" t="s">
         <v>99</v>
       </c>
+      <c r="C48" t="s">
+        <v>184</v>
+      </c>
       <c r="D48" t="s">
         <v>10</v>
       </c>
@@ -1648,6 +2030,9 @@
       <c r="B49" t="s">
         <v>101</v>
       </c>
+      <c r="C49" t="s">
+        <v>185</v>
+      </c>
       <c r="D49" t="s">
         <v>10</v>
       </c>
@@ -1664,6 +2049,9 @@
       </c>
       <c r="B50" t="s">
         <v>103</v>
+      </c>
+      <c r="C50" t="s">
+        <v>186</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
@@ -1682,6 +2070,9 @@
       <c r="B51" t="s">
         <v>105</v>
       </c>
+      <c r="C51" t="s">
+        <v>187</v>
+      </c>
       <c r="D51" t="s">
         <v>10</v>
       </c>
@@ -1699,6 +2090,9 @@
       <c r="B52" t="s">
         <v>106</v>
       </c>
+      <c r="C52" t="s">
+        <v>188</v>
+      </c>
       <c r="D52" t="s">
         <v>10</v>
       </c>
@@ -1716,6 +2110,9 @@
       <c r="B53" t="s">
         <v>107</v>
       </c>
+      <c r="C53" t="s">
+        <v>189</v>
+      </c>
       <c r="D53" t="s">
         <v>10</v>
       </c>
@@ -1733,6 +2130,9 @@
       <c r="B54" t="s">
         <v>108</v>
       </c>
+      <c r="C54" t="s">
+        <v>190</v>
+      </c>
       <c r="D54" t="s">
         <v>10</v>
       </c>
@@ -1750,6 +2150,9 @@
       <c r="B55" t="s">
         <v>109</v>
       </c>
+      <c r="C55" t="s">
+        <v>191</v>
+      </c>
       <c r="D55" t="s">
         <v>10</v>
       </c>
@@ -1767,6 +2170,9 @@
       <c r="B56" t="s">
         <v>115</v>
       </c>
+      <c r="C56" t="s">
+        <v>192</v>
+      </c>
       <c r="D56" t="s">
         <v>10</v>
       </c>
@@ -1784,6 +2190,9 @@
       <c r="B57" t="s">
         <v>116</v>
       </c>
+      <c r="C57" t="s">
+        <v>193</v>
+      </c>
       <c r="D57" t="s">
         <v>10</v>
       </c>
@@ -1801,6 +2210,9 @@
       <c r="B58" t="s">
         <v>117</v>
       </c>
+      <c r="C58" t="s">
+        <v>194</v>
+      </c>
       <c r="D58" t="s">
         <v>10</v>
       </c>
@@ -1818,6 +2230,9 @@
       <c r="B59" t="s">
         <v>118</v>
       </c>
+      <c r="C59" t="s">
+        <v>195</v>
+      </c>
       <c r="D59" t="s">
         <v>10</v>
       </c>
@@ -1835,6 +2250,9 @@
       <c r="B60" t="s">
         <v>123</v>
       </c>
+      <c r="C60" t="s">
+        <v>196</v>
+      </c>
       <c r="D60" t="s">
         <v>10</v>
       </c>
@@ -1852,6 +2270,9 @@
       <c r="B61" t="s">
         <v>124</v>
       </c>
+      <c r="C61" t="s">
+        <v>197</v>
+      </c>
       <c r="D61" t="s">
         <v>10</v>
       </c>
@@ -1869,6 +2290,9 @@
       <c r="B62" t="s">
         <v>127</v>
       </c>
+      <c r="C62" t="s">
+        <v>198</v>
+      </c>
       <c r="D62" t="s">
         <v>10</v>
       </c>
@@ -1886,6 +2310,9 @@
       <c r="B63" t="s">
         <v>128</v>
       </c>
+      <c r="C63" t="s">
+        <v>199</v>
+      </c>
       <c r="D63" t="s">
         <v>10</v>
       </c>
@@ -1903,6 +2330,9 @@
       <c r="B64" t="s">
         <v>129</v>
       </c>
+      <c r="C64" t="s">
+        <v>200</v>
+      </c>
       <c r="D64" t="s">
         <v>10</v>
       </c>
@@ -1920,6 +2350,9 @@
       <c r="B65" t="s">
         <v>133</v>
       </c>
+      <c r="C65" t="s">
+        <v>201</v>
+      </c>
       <c r="D65" t="s">
         <v>10</v>
       </c>
@@ -1937,6 +2370,9 @@
       <c r="B66" t="s">
         <v>134</v>
       </c>
+      <c r="C66" t="s">
+        <v>202</v>
+      </c>
       <c r="D66" t="s">
         <v>10</v>
       </c>
@@ -1944,6 +2380,86 @@
         <v>136</v>
       </c>
       <c r="F66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1988</v>
+      </c>
+      <c r="B67" t="s">
+        <v>203</v>
+      </c>
+      <c r="C67" t="s">
+        <v>207</v>
+      </c>
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>205</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1989</v>
+      </c>
+      <c r="B68" t="s">
+        <v>204</v>
+      </c>
+      <c r="C68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>206</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1988</v>
+      </c>
+      <c r="B69" t="s">
+        <v>209</v>
+      </c>
+      <c r="C69" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>213</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1990</v>
+      </c>
+      <c r="B70" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" t="s">
+        <v>212</v>
+      </c>
+      <c r="D70" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" t="s">
+        <v>214</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more famicon adv books
</commit_message>
<xml_diff>
--- a/famicon-adventure-gamebook/checklist.xlsx
+++ b/famicon-adventure-gamebook/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/famicon-adventure-gamebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2044E66-89F6-6443-82AB-5580AD761BB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{534F32BE-DBCB-4945-809E-A910451D4BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{34C05C4E-05DE-9C4D-BAF0-7EC06EA20153}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="293">
   <si>
     <t>year</t>
   </si>
@@ -814,6 +814,105 @@
   </si>
   <si>
     <t>jaseiken-necromancer.jpg</t>
+  </si>
+  <si>
+    <t>space_time_pirates.jpeg</t>
+  </si>
+  <si>
+    <t>超時空パイレーツ おみそれ3人組の冒険</t>
+  </si>
+  <si>
+    <t>Super Space Time Pirates</t>
+  </si>
+  <si>
+    <t>トキメキハイスクール 恋の学園祭大作戦</t>
+  </si>
+  <si>
+    <t>Tokimeki High School</t>
+  </si>
+  <si>
+    <t>tokimeki_high_school.jpeg</t>
+  </si>
+  <si>
+    <t>霊幻道士 キョンシー大戦争</t>
+  </si>
+  <si>
+    <t>Mr. Vampire Jiangshi Great War</t>
+  </si>
+  <si>
+    <t>mr_vampire.jpeg</t>
+  </si>
+  <si>
+    <t>ガイアの紋章 エルスリード英雄列伝</t>
+  </si>
+  <si>
+    <t>Gaia's Coat of Arms</t>
+  </si>
+  <si>
+    <t>gaias_coat_of_arms.jpg</t>
+  </si>
+  <si>
+    <t>visit_yamato_genie.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ヤマト魔神伝 サギリ見参! </t>
+  </si>
+  <si>
+    <t>Visit Yamato Genie</t>
+  </si>
+  <si>
+    <t>deep_dungeon_3.jpeg</t>
+  </si>
+  <si>
+    <t>ディープダンジョンIII</t>
+  </si>
+  <si>
+    <t>Deep Dungeon III</t>
+  </si>
+  <si>
+    <t>dragon_rock.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ドラゴンロック 浮遊要塞の死闘 </t>
+  </si>
+  <si>
+    <t>Dragon Rock</t>
+  </si>
+  <si>
+    <t>genpei_tomaden.jpeg</t>
+  </si>
+  <si>
+    <t>Genpei Tomaden</t>
+  </si>
+  <si>
+    <t>源平討魔伝 神異妖魔界の変</t>
+  </si>
+  <si>
+    <t>dark_fortress_guardian.jpg</t>
+  </si>
+  <si>
+    <t>Dark Fortress Guardian</t>
+  </si>
+  <si>
+    <t>暗黒要塞ガルディアン オセロ神話の謎</t>
+  </si>
+  <si>
+    <t>kaiju_monogatari.jpeg</t>
+  </si>
+  <si>
+    <t>Kaiju Monogatari</t>
+  </si>
+  <si>
+    <t>貝獣物語 シェルドラド伝説</t>
+  </si>
+  <si>
+    <t>space_harrier.jpeg</t>
+  </si>
+  <si>
+    <t>スペース・ハリアー ホワイトドラゴンの勇者</t>
+  </si>
+  <si>
+    <t>Space Harrier</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B05840-0655-A245-99C3-6C443B4A591B}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84:F85"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85:F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,6 +2997,226 @@
         <v>11</v>
       </c>
     </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1988</v>
+      </c>
+      <c r="B86" t="s">
+        <v>261</v>
+      </c>
+      <c r="C86" t="s">
+        <v>262</v>
+      </c>
+      <c r="D86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" t="s">
+        <v>260</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1988</v>
+      </c>
+      <c r="B87" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" t="s">
+        <v>264</v>
+      </c>
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" t="s">
+        <v>265</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1988</v>
+      </c>
+      <c r="B88" t="s">
+        <v>266</v>
+      </c>
+      <c r="C88" t="s">
+        <v>267</v>
+      </c>
+      <c r="D88" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" t="s">
+        <v>268</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1988</v>
+      </c>
+      <c r="B89" t="s">
+        <v>269</v>
+      </c>
+      <c r="C89" t="s">
+        <v>270</v>
+      </c>
+      <c r="D89" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" t="s">
+        <v>271</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1988</v>
+      </c>
+      <c r="B90" t="s">
+        <v>273</v>
+      </c>
+      <c r="C90" t="s">
+        <v>274</v>
+      </c>
+      <c r="D90" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" t="s">
+        <v>272</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1988</v>
+      </c>
+      <c r="B91" t="s">
+        <v>276</v>
+      </c>
+      <c r="C91" t="s">
+        <v>277</v>
+      </c>
+      <c r="D91" t="s">
+        <v>10</v>
+      </c>
+      <c r="E91" t="s">
+        <v>275</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1988</v>
+      </c>
+      <c r="B92" t="s">
+        <v>279</v>
+      </c>
+      <c r="C92" t="s">
+        <v>280</v>
+      </c>
+      <c r="D92" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" t="s">
+        <v>278</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1988</v>
+      </c>
+      <c r="B93" t="s">
+        <v>283</v>
+      </c>
+      <c r="C93" t="s">
+        <v>282</v>
+      </c>
+      <c r="D93" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" t="s">
+        <v>281</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1988</v>
+      </c>
+      <c r="B94" t="s">
+        <v>286</v>
+      </c>
+      <c r="C94" t="s">
+        <v>285</v>
+      </c>
+      <c r="D94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" t="s">
+        <v>284</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1988</v>
+      </c>
+      <c r="B95" t="s">
+        <v>289</v>
+      </c>
+      <c r="C95" t="s">
+        <v>288</v>
+      </c>
+      <c r="D95" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" t="s">
+        <v>287</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1988</v>
+      </c>
+      <c r="B96" t="s">
+        <v>291</v>
+      </c>
+      <c r="C96" t="s">
+        <v>292</v>
+      </c>
+      <c r="D96" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" t="s">
+        <v>290</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>